<commit_message>
These are the changes which is done w.t.t MD approval flow implementation
</commit_message>
<xml_diff>
--- a/Acro_Data_Driven_Framework/Acams_Suite_One.xlsx
+++ b/Acro_Data_Driven_Framework/Acams_Suite_One.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11655" windowHeight="4650" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11655" windowHeight="4650"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="152">
   <si>
     <t>TCID</t>
   </si>
@@ -444,9 +444,6 @@
     <t>CMS Only</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>greg.bergman</t>
   </si>
   <si>
@@ -468,7 +465,13 @@
     <t>201712018768</t>
   </si>
   <si>
-    <t xml:space="preserve">201712018777 </t>
+    <t xml:space="preserve">201712018811 </t>
+  </si>
+  <si>
+    <t>MdApprovalComment</t>
+  </si>
+  <si>
+    <t>ABCD</t>
   </si>
 </sst>
 </file>
@@ -524,7 +527,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -584,11 +587,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -623,7 +635,10 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -930,8 +945,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -953,7 +968,7 @@
         <v>129</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>142</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1006,8 +1021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AS102"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView topLeftCell="A93" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I107" sqref="I107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1086,7 +1101,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D3" s="12" t="s">
         <v>110</v>
@@ -1260,11 +1275,11 @@
         <v>18</v>
       </c>
       <c r="J7" s="15" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="K7" s="9"/>
       <c r="L7" s="15" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="M7" s="1" t="s">
         <v>122</v>
@@ -1622,7 +1637,7 @@
         <v>130</v>
       </c>
       <c r="W13" s="15" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="X13" s="1" t="s">
         <v>57</v>
@@ -1646,13 +1661,13 @@
         <v>59</v>
       </c>
       <c r="AE13" t="s">
+        <v>145</v>
+      </c>
+      <c r="AF13" t="s">
         <v>146</v>
       </c>
-      <c r="AF13" t="s">
+      <c r="AG13" t="s">
         <v>147</v>
-      </c>
-      <c r="AG13" t="s">
-        <v>148</v>
       </c>
     </row>
     <row r="14" spans="1:45" x14ac:dyDescent="0.25">
@@ -1759,13 +1774,13 @@
         <v>6</v>
       </c>
       <c r="C19" t="s">
+        <v>145</v>
+      </c>
+      <c r="D19" t="s">
         <v>146</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>147</v>
-      </c>
-      <c r="E19" t="s">
-        <v>148</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>48</v>
@@ -1872,13 +1887,13 @@
         <v>6</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D24" t="s">
+        <v>146</v>
+      </c>
+      <c r="E24" t="s">
         <v>147</v>
-      </c>
-      <c r="E24" t="s">
-        <v>148</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>138</v>
@@ -1915,7 +1930,7 @@
       <c r="L25" s="21"/>
       <c r="M25" s="21"/>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="8" t="s">
         <v>129</v>
       </c>
@@ -1924,7 +1939,7 @@
       <c r="G100" s="11"/>
       <c r="H100" s="11"/>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101" s="4" t="s">
         <v>1</v>
       </c>
@@ -1949,8 +1964,11 @@
       <c r="H101" s="6" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I101" s="17" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
         <v>2</v>
       </c>
@@ -1958,7 +1976,7 @@
         <v>6</v>
       </c>
       <c r="C102" s="16" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D102" t="s">
         <v>100</v>
@@ -1974,6 +1992,9 @@
       </c>
       <c r="H102" s="1" t="s">
         <v>81</v>
+      </c>
+      <c r="I102" s="23" t="s">
+        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Eligibility Changes done 12/27/2017
Signed-off-by: ACROTECHNOLOGIE\SSinghal <sarthak.singhal8723@gmail.com>
</commit_message>
<xml_diff>
--- a/Acro_Data_Driven_Framework/Acams_Suite_One.xlsx
+++ b/Acro_Data_Driven_Framework/Acams_Suite_One.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11655" windowHeight="4650"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11655" windowHeight="4650" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="155">
   <si>
     <t>TCID</t>
   </si>
@@ -450,35 +450,45 @@
     <t>John</t>
   </si>
   <si>
-    <t>Waltson</t>
-  </si>
-  <si>
-    <t>201712018789</t>
-  </si>
-  <si>
-    <t>20171204000194</t>
-  </si>
-  <si>
-    <t>Waltson, John</t>
-  </si>
-  <si>
-    <t>201712018768</t>
-  </si>
-  <si>
-    <t xml:space="preserve">201712018811 </t>
-  </si>
-  <si>
     <t>MdApprovalComment</t>
   </si>
   <si>
     <t>ABCD</t>
+  </si>
+  <si>
+    <t>201712018819</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>201712018823</t>
+  </si>
+  <si>
+    <t>20171204000246</t>
+  </si>
+  <si>
+    <t>Cena, John</t>
+  </si>
+  <si>
+    <t>Saamuel</t>
+  </si>
+  <si>
+    <t>201712018824</t>
+  </si>
+  <si>
+    <t>20171204000247</t>
+  </si>
+  <si>
+    <t>Saamuel, John</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -600,7 +610,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -625,7 +635,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -635,9 +644,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -945,14 +951,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="48.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="25.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -968,7 +974,7 @@
         <v>129</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
+        <v>147</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1021,54 +1027,54 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AS102"/>
   <sheetViews>
-    <sheetView topLeftCell="A93" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I107" sqref="I107"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W13" sqref="W13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="15.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="38.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="44" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="29.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="17.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="34.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="15.85546875" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="44.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="26.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="20.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="21.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="25.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="36.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="24.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="23" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="25.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="24.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="5.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="7.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="30.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="38.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="44.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="29.28515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="17.140625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="34.5703125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="44.28515625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="26.42578125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="20.5703125" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="21.140625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="25.7109375" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="36.7109375" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="24.28515625" collapsed="true"/>
+    <col min="22" max="23" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="25.7109375" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="24.28515625" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="36" max="36" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="37" max="37" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
+    <col min="38" max="38" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="39" max="39" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="40" max="40" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
+    <col min="41" max="41" bestFit="true" customWidth="true" width="5.85546875" collapsed="true"/>
+    <col min="42" max="42" bestFit="true" customWidth="true" width="7.7109375" collapsed="true"/>
+    <col min="43" max="43" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:45" x14ac:dyDescent="0.25">
@@ -1279,7 +1285,7 @@
       </c>
       <c r="K7" s="9"/>
       <c r="L7" s="15" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="M7" s="1" t="s">
         <v>122</v>
@@ -1637,7 +1643,7 @@
         <v>130</v>
       </c>
       <c r="W13" s="15" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
       <c r="X13" s="1" t="s">
         <v>57</v>
@@ -1661,13 +1667,13 @@
         <v>59</v>
       </c>
       <c r="AE13" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="AF13" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="AG13" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
     </row>
     <row r="14" spans="1:45" x14ac:dyDescent="0.25">
@@ -1711,58 +1717,58 @@
       </c>
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A18" s="19" t="s">
+      <c r="A18" s="18" t="s">
         <v>1</v>
       </c>
-      <c r="B18" s="20" t="s">
+      <c r="B18" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="20" t="s">
+      <c r="C18" s="19" t="s">
         <v>73</v>
       </c>
-      <c r="D18" s="20" t="s">
+      <c r="D18" s="19" t="s">
         <v>74</v>
       </c>
-      <c r="E18" s="20" t="s">
+      <c r="E18" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="F18" s="20" t="s">
+      <c r="F18" s="19" t="s">
         <v>75</v>
       </c>
-      <c r="G18" s="19" t="s">
+      <c r="G18" s="18" t="s">
         <v>76</v>
       </c>
-      <c r="H18" s="19" t="s">
+      <c r="H18" s="18" t="s">
         <v>77</v>
       </c>
-      <c r="I18" s="20" t="s">
+      <c r="I18" s="19" t="s">
         <v>78</v>
       </c>
-      <c r="J18" s="19" t="s">
+      <c r="J18" s="18" t="s">
         <v>126</v>
       </c>
-      <c r="K18" s="20" t="s">
+      <c r="K18" s="19" t="s">
         <v>127</v>
       </c>
-      <c r="L18" s="19" t="s">
+      <c r="L18" s="18" t="s">
         <v>132</v>
       </c>
-      <c r="M18" s="20" t="s">
+      <c r="M18" s="19" t="s">
         <v>84</v>
       </c>
-      <c r="N18" s="17" t="s">
+      <c r="N18" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="O18" s="18" t="s">
+      <c r="O18" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="P18" s="17" t="s">
+      <c r="P18" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="Q18" s="18" t="s">
+      <c r="Q18" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="R18" s="17" t="s">
+      <c r="R18" s="16" t="s">
         <v>98</v>
       </c>
     </row>
@@ -1774,13 +1780,13 @@
         <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>145</v>
+        <v>152</v>
       </c>
       <c r="D19" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="E19" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>48</v>
@@ -1886,14 +1892,14 @@
       <c r="B24" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C24" s="22" t="s">
-        <v>149</v>
+      <c r="C24" t="s">
+        <v>152</v>
       </c>
       <c r="D24" t="s">
-        <v>146</v>
+        <v>153</v>
       </c>
       <c r="E24" t="s">
-        <v>147</v>
+        <v>154</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>138</v>
@@ -1922,13 +1928,13 @@
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
       <c r="F25" s="1"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="21"/>
-      <c r="I25" s="21"/>
-      <c r="J25" s="21"/>
-      <c r="K25" s="21"/>
-      <c r="L25" s="21"/>
-      <c r="M25" s="21"/>
+      <c r="G25" s="20"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
+      <c r="J25" s="20"/>
+      <c r="K25" s="20"/>
+      <c r="L25" s="20"/>
+      <c r="M25" s="20"/>
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="8" t="s">
@@ -1964,8 +1970,8 @@
       <c r="H101" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="I101" s="17" t="s">
-        <v>150</v>
+      <c r="I101" s="16" t="s">
+        <v>144</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
@@ -1975,8 +1981,8 @@
       <c r="B102" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C102" s="16" t="s">
-        <v>148</v>
+      <c r="C102" t="s">
+        <v>146</v>
       </c>
       <c r="D102" t="s">
         <v>100</v>
@@ -1993,8 +1999,8 @@
       <c r="H102" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="I102" s="23" t="s">
-        <v>151</v>
+      <c r="I102" s="21" t="s">
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -2007,50 +2013,50 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO31"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A64" workbookViewId="0">
       <selection activeCell="A33" sqref="A33:XFD36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="27" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="31.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="5.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="7.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="7.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="6" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="8.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="8.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="4.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="5.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="39.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="8.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="20.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="27.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="31.7109375" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="8.5703125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="5.85546875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="7.7109375" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="7.140625" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="6.0" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="8.5703125" collapsed="true"/>
+    <col min="36" max="36" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="37" max="37" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="38" max="38" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="39" max="39" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="40" max="40" bestFit="true" customWidth="true" width="4.5703125" collapsed="true"/>
+    <col min="41" max="41" bestFit="true" customWidth="true" width="5.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:41" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Adding the CMS Card Class file
Signed-off-by: ACROTECHNOLOGIE\SSinghal <sarthak.singhal8723@gmail.com>
</commit_message>
<xml_diff>
--- a/Acro_Data_Driven_Framework/Acams_Suite_One.xlsx
+++ b/Acro_Data_Driven_Framework/Acams_Suite_One.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="156">
   <si>
     <t>TCID</t>
   </si>
@@ -447,9 +447,6 @@
     <t>greg.bergman</t>
   </si>
   <si>
-    <t>John</t>
-  </si>
-  <si>
     <t>MdApprovalComment</t>
   </si>
   <si>
@@ -462,18 +459,6 @@
     <t>N</t>
   </si>
   <si>
-    <t>201712018823</t>
-  </si>
-  <si>
-    <t>20171204000246</t>
-  </si>
-  <si>
-    <t>Cena, John</t>
-  </si>
-  <si>
-    <t>Saamuel</t>
-  </si>
-  <si>
     <t>201712018824</t>
   </si>
   <si>
@@ -481,6 +466,24 @@
   </si>
   <si>
     <t>Saamuel, John</t>
+  </si>
+  <si>
+    <t>CMS_Card_Test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I am approving the ICD code </t>
+  </si>
+  <si>
+    <t xml:space="preserve">James </t>
+  </si>
+  <si>
+    <t>201712018825</t>
+  </si>
+  <si>
+    <t>20171204000248</t>
+  </si>
+  <si>
+    <t>Race, James</t>
   </si>
 </sst>
 </file>
@@ -505,7 +508,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -533,6 +536,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -610,7 +625,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -645,6 +660,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -949,10 +966,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -970,11 +987,11 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="22" t="s">
         <v>129</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>147</v>
+      <c r="B2" s="22" t="s">
+        <v>146</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -1016,6 +1033,18 @@
       <c r="B7" s="13" t="s">
         <v>2</v>
       </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="23" t="s">
+        <v>150</v>
+      </c>
+      <c r="B8" s="23" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1027,7 +1056,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AS102"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="P1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="W13" sqref="W13"/>
     </sheetView>
   </sheetViews>
@@ -1281,11 +1310,11 @@
         <v>18</v>
       </c>
       <c r="J7" s="15" t="s">
-        <v>143</v>
+        <v>152</v>
       </c>
       <c r="K7" s="9"/>
       <c r="L7" s="15" t="s">
-        <v>151</v>
+        <v>22</v>
       </c>
       <c r="M7" s="1" t="s">
         <v>122</v>
@@ -1643,7 +1672,7 @@
         <v>130</v>
       </c>
       <c r="W13" s="15" t="s">
-        <v>151</v>
+        <v>22</v>
       </c>
       <c r="X13" s="1" t="s">
         <v>57</v>
@@ -1667,13 +1696,13 @@
         <v>59</v>
       </c>
       <c r="AE13" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="AF13" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="AG13" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
     </row>
     <row r="14" spans="1:45" x14ac:dyDescent="0.25">
@@ -1780,13 +1809,13 @@
         <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D19" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E19" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>48</v>
@@ -1874,7 +1903,9 @@
       <c r="H23" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="I23" s="6"/>
+      <c r="I23" s="6" t="s">
+        <v>143</v>
+      </c>
       <c r="J23" s="4"/>
       <c r="K23" s="6"/>
       <c r="L23" s="4"/>
@@ -1893,13 +1924,13 @@
         <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="D24" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="E24" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>138</v>
@@ -1910,7 +1941,9 @@
       <c r="H24" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="I24" s="1"/>
+      <c r="I24" s="1" t="s">
+        <v>151</v>
+      </c>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
       <c r="L24" s="9"/>
@@ -1936,6 +1969,84 @@
       <c r="L25" s="20"/>
       <c r="M25" s="20"/>
     </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B29" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="4"/>
+      <c r="M29" s="6"/>
+      <c r="N29" s="4"/>
+      <c r="O29" s="6"/>
+      <c r="P29" s="4"/>
+      <c r="Q29" s="6"/>
+      <c r="R29" s="4"/>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" t="s">
+        <v>153</v>
+      </c>
+      <c r="D30" t="s">
+        <v>154</v>
+      </c>
+      <c r="E30" t="s">
+        <v>155</v>
+      </c>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="9"/>
+      <c r="M30" s="1"/>
+      <c r="N30" s="9"/>
+      <c r="O30" s="9"/>
+      <c r="P30" s="9"/>
+      <c r="Q30" s="9"/>
+      <c r="R30" s="9"/>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="20"/>
+      <c r="I31" s="20"/>
+      <c r="J31" s="20"/>
+      <c r="K31" s="20"/>
+      <c r="L31" s="20"/>
+      <c r="M31" s="20"/>
+    </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100" s="8" t="s">
         <v>129</v>
@@ -1971,7 +2082,7 @@
         <v>78</v>
       </c>
       <c r="I101" s="16" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
@@ -1982,7 +2093,7 @@
         <v>6</v>
       </c>
       <c r="C102" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D102" t="s">
         <v>100</v>
@@ -2000,7 +2111,7 @@
         <v>81</v>
       </c>
       <c r="I102" s="21" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CMS card Test Case 10 and 11
Signed-off-by: ACROTECHNOLOGIE\SSinghal <sarthak.singhal8723@gmail.com>
</commit_message>
<xml_diff>
--- a/Acro_Data_Driven_Framework/Acams_Suite_One.xlsx
+++ b/Acro_Data_Driven_Framework/Acams_Suite_One.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="333" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="159">
   <si>
     <t>TCID</t>
   </si>
@@ -450,28 +450,49 @@
     <t>MdApprovalComment</t>
   </si>
   <si>
+    <t>CMS_Card_Test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I am approving the ICD code </t>
+  </si>
+  <si>
+    <t>201801000467</t>
+  </si>
+  <si>
+    <t>20180104000480</t>
+  </si>
+  <si>
+    <t>Acams, CMS</t>
+  </si>
+  <si>
     <t>N</t>
   </si>
   <si>
-    <t>CMS_Card_Test</t>
-  </si>
-  <si>
-    <t xml:space="preserve">I am approving the ICD code </t>
-  </si>
-  <si>
-    <t>CMS</t>
-  </si>
-  <si>
-    <t>Acams</t>
-  </si>
-  <si>
-    <t>201801000467</t>
-  </si>
-  <si>
-    <t>20180104000480</t>
-  </si>
-  <si>
-    <t>Acams, CMS</t>
+    <t>201801000960</t>
+  </si>
+  <si>
+    <t>20180104001044</t>
+  </si>
+  <si>
+    <t>Marathon, James</t>
+  </si>
+  <si>
+    <t>Tailor, John</t>
+  </si>
+  <si>
+    <t>John</t>
+  </si>
+  <si>
+    <t>Tailor</t>
+  </si>
+  <si>
+    <t>ReferralClientName</t>
+  </si>
+  <si>
+    <t>Jordon</t>
+  </si>
+  <si>
+    <t>James</t>
   </si>
 </sst>
 </file>
@@ -495,7 +516,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -523,12 +544,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF00B0F0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -603,7 +618,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -638,7 +653,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -946,7 +960,7 @@
   <dimension ref="A1:B8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="L5" sqref="L5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -972,51 +986,51 @@
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="21" t="s">
         <v>109</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="21" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
+      <c r="A4" s="21" t="s">
         <v>114</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="21" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="22" t="s">
+      <c r="A5" s="21" t="s">
         <v>20</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="21" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="22" t="s">
+      <c r="A6" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="21" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="22" t="s">
+      <c r="A7" s="21" t="s">
         <v>136</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="21" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="21" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>144</v>
+        <v>2</v>
       </c>
     </row>
   </sheetData>
@@ -1027,10 +1041,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AS102"/>
+  <dimension ref="A1:AS35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B94" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F102" sqref="F102"/>
+    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1067,7 +1081,7 @@
     <col min="31" max="31" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="32" max="32" width="24.28515625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="33" max="33" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="34" max="34" width="26.28515625" customWidth="1" collapsed="1"/>
     <col min="35" max="35" width="18" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="36" max="36" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="37" max="37" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
@@ -1283,11 +1297,11 @@
         <v>18</v>
       </c>
       <c r="J7" s="14" t="s">
-        <v>147</v>
+        <v>158</v>
       </c>
       <c r="K7" s="9"/>
       <c r="L7" s="14" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="M7" s="1" t="s">
         <v>122</v>
@@ -1576,6 +1590,9 @@
       <c r="AG12" s="6" t="s">
         <v>128</v>
       </c>
+      <c r="AH12" s="6" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="13" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
@@ -1645,7 +1662,7 @@
         <v>130</v>
       </c>
       <c r="W13" s="14" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
       <c r="X13" s="1" t="s">
         <v>57</v>
@@ -1669,13 +1686,13 @@
         <v>59</v>
       </c>
       <c r="AE13" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="AF13" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="AG13" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
     </row>
     <row r="14" spans="1:45" x14ac:dyDescent="0.25">
@@ -1782,13 +1799,13 @@
         <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D19" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E19" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>48</v>
@@ -1891,19 +1908,19 @@
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>2</v>
+        <v>149</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D24" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E24" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>138</v>
@@ -1915,7 +1932,7 @@
         <v>141</v>
       </c>
       <c r="I24" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="J24" s="1"/>
       <c r="K24" s="1"/>
@@ -1944,7 +1961,7 @@
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.25">
@@ -1960,7 +1977,9 @@
       <c r="D29" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="E29" s="6"/>
+      <c r="E29" s="6" t="s">
+        <v>128</v>
+      </c>
       <c r="F29" s="6"/>
       <c r="G29" s="4"/>
       <c r="H29" s="4"/>
@@ -1983,13 +2002,13 @@
         <v>6</v>
       </c>
       <c r="C30" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="D30" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="E30" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
@@ -2020,72 +2039,82 @@
       <c r="L31" s="19"/>
       <c r="M31" s="19"/>
     </row>
-    <row r="100" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A100" s="8" t="s">
+    <row r="33" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
         <v>129</v>
       </c>
-      <c r="E100" s="11"/>
-      <c r="F100" s="11"/>
-      <c r="G100" s="11"/>
-      <c r="H100" s="11"/>
-    </row>
-    <row r="101" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A101" s="4" t="s">
+      <c r="E33" s="11"/>
+      <c r="F33" s="11"/>
+      <c r="G33" s="11"/>
+      <c r="H33" s="11"/>
+    </row>
+    <row r="34" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="B101" s="6" t="s">
+      <c r="B34" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C101" s="6" t="s">
+      <c r="C34" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="D101" s="6" t="s">
+      <c r="D34" s="6" t="s">
         <v>74</v>
       </c>
-      <c r="E101" s="6"/>
-      <c r="F101" s="6"/>
-      <c r="G101" s="4"/>
-      <c r="H101" s="4"/>
-      <c r="I101" s="6"/>
-      <c r="J101" s="4"/>
-      <c r="K101" s="6"/>
-      <c r="L101" s="4"/>
-      <c r="M101" s="6"/>
-      <c r="N101" s="4"/>
-      <c r="O101" s="6"/>
-      <c r="P101" s="4"/>
-      <c r="Q101" s="6"/>
-      <c r="R101" s="4"/>
-    </row>
-    <row r="102" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A102" s="1" t="s">
+      <c r="E34" s="6" t="s">
+        <v>128</v>
+      </c>
+      <c r="F34" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="H34" s="4"/>
+      <c r="I34" s="6"/>
+      <c r="J34" s="4"/>
+      <c r="K34" s="6"/>
+      <c r="L34" s="4"/>
+      <c r="M34" s="6"/>
+      <c r="N34" s="4"/>
+      <c r="O34" s="6"/>
+      <c r="P34" s="4"/>
+      <c r="Q34" s="6"/>
+      <c r="R34" s="4"/>
+    </row>
+    <row r="35" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B102" s="1" t="s">
+      <c r="B35" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C102" t="s">
-        <v>149</v>
-      </c>
-      <c r="D102" t="s">
-        <v>150</v>
-      </c>
-      <c r="E102" t="s">
-        <v>151</v>
-      </c>
-      <c r="F102" s="1"/>
-      <c r="G102" s="1"/>
-      <c r="H102" s="1"/>
-      <c r="I102" s="1"/>
-      <c r="J102" s="1"/>
-      <c r="K102" s="1"/>
-      <c r="L102" s="9"/>
-      <c r="M102" s="1"/>
-      <c r="N102" s="9"/>
-      <c r="O102" s="9"/>
-      <c r="P102" s="9"/>
-      <c r="Q102" s="9"/>
-      <c r="R102" s="9"/>
+      <c r="C35" t="s">
+        <v>146</v>
+      </c>
+      <c r="D35" t="s">
+        <v>147</v>
+      </c>
+      <c r="E35" t="s">
+        <v>148</v>
+      </c>
+      <c r="F35" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="G35" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+      <c r="L35" s="9"/>
+      <c r="M35" s="1"/>
+      <c r="N35" s="9"/>
+      <c r="O35" s="9"/>
+      <c r="P35" s="9"/>
+      <c r="Q35" s="9"/>
+      <c r="R35" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
CMS card Last Test CAse
Signed-off-by: ACROTECHNOLOGIE\SSinghal <sarthak.singhal8723@gmail.com>
</commit_message>
<xml_diff>
--- a/Acro_Data_Driven_Framework/Acams_Suite_One.xlsx
+++ b/Acro_Data_Driven_Framework/Acams_Suite_One.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11655" windowHeight="4650" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11655" windowHeight="4650"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="339" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="340" uniqueCount="157">
   <si>
     <t>TCID</t>
   </si>
@@ -459,21 +459,6 @@
     <t>Acams, CMS</t>
   </si>
   <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>201801000960</t>
-  </si>
-  <si>
-    <t>20180104001044</t>
-  </si>
-  <si>
-    <t>Marathon, James</t>
-  </si>
-  <si>
-    <t>Tailor, John</t>
-  </si>
-  <si>
     <t>John</t>
   </si>
   <si>
@@ -483,13 +468,25 @@
     <t>ReferralClientName</t>
   </si>
   <si>
-    <t>Jordon</t>
-  </si>
-  <si>
     <t>James</t>
   </si>
   <si>
     <t>greg.bergman</t>
+  </si>
+  <si>
+    <t>1234</t>
+  </si>
+  <si>
+    <t>Morathan</t>
+  </si>
+  <si>
+    <t>201801000977</t>
+  </si>
+  <si>
+    <t>20180104001066</t>
+  </si>
+  <si>
+    <t>Morathan, James</t>
   </si>
 </sst>
 </file>
@@ -956,8 +953,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1040,8 +1037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AS35"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1120,10 +1117,10 @@
         <v>6</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>157</v>
-      </c>
-      <c r="D3" s="12">
-        <v>1234</v>
+        <v>151</v>
+      </c>
+      <c r="D3" s="12" t="s">
+        <v>152</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>2</v>
@@ -1294,11 +1291,11 @@
         <v>18</v>
       </c>
       <c r="J7" s="14" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="K7" s="9"/>
       <c r="L7" s="14" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="M7" s="1" t="s">
         <v>121</v>
@@ -1588,7 +1585,7 @@
         <v>127</v>
       </c>
       <c r="AH12" s="6" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13" spans="1:45" x14ac:dyDescent="0.25">
@@ -1659,7 +1656,7 @@
         <v>129</v>
       </c>
       <c r="W13" s="14" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="X13" s="1" t="s">
         <v>57</v>
@@ -1683,13 +1680,13 @@
         <v>59</v>
       </c>
       <c r="AE13" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="AF13" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="AG13" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
     </row>
     <row r="14" spans="1:45" x14ac:dyDescent="0.25">
@@ -1796,13 +1793,13 @@
         <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="D19" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="E19" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>48</v>
@@ -1905,19 +1902,19 @@
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>147</v>
+        <v>2</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="D24" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="E24" t="s">
-        <v>150</v>
+        <v>156</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>137</v>
@@ -1999,13 +1996,13 @@
         <v>6</v>
       </c>
       <c r="C30" t="s">
-        <v>148</v>
+        <v>154</v>
       </c>
       <c r="D30" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="E30" t="s">
-        <v>151</v>
+        <v>156</v>
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
@@ -2096,10 +2093,10 @@
         <v>146</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>

</xml_diff>

<commit_message>
PA 309 test case creation
Signed-off-by: ACROTECHNOLOGIE\SSinghal <sarthak.singhal8723@gmail.com>
</commit_message>
<xml_diff>
--- a/Acro_Data_Driven_Framework/Acams_Suite_One.xlsx
+++ b/Acro_Data_Driven_Framework/Acams_Suite_One.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="167">
   <si>
     <t>TCID</t>
   </si>
@@ -468,31 +468,55 @@
     <t>1234</t>
   </si>
   <si>
-    <t>Janis</t>
-  </si>
-  <si>
     <t>678-90-8765</t>
   </si>
   <si>
     <t>Gonzalwis, Janis</t>
   </si>
   <si>
-    <t>201801002639</t>
-  </si>
-  <si>
-    <t>20180104005194</t>
-  </si>
-  <si>
-    <t>Jenilivia</t>
-  </si>
-  <si>
-    <t>201801002647</t>
-  </si>
-  <si>
-    <t>20180104005203</t>
-  </si>
-  <si>
-    <t>Jenilivia, Janis</t>
+    <t>PA309_Test</t>
+  </si>
+  <si>
+    <t>ProviderName</t>
+  </si>
+  <si>
+    <t>180 MEDICAL INC</t>
+  </si>
+  <si>
+    <t>Insurance Name</t>
+  </si>
+  <si>
+    <t>FinalComments</t>
+  </si>
+  <si>
+    <t>PA309 created</t>
+  </si>
+  <si>
+    <t>201802002664</t>
+  </si>
+  <si>
+    <t>20180204000001</t>
+  </si>
+  <si>
+    <t>Jennifer, Janis</t>
+  </si>
+  <si>
+    <t>Henry</t>
+  </si>
+  <si>
+    <t>Johnathann</t>
+  </si>
+  <si>
+    <t>Johnathan</t>
+  </si>
+  <si>
+    <t>201802002665</t>
+  </si>
+  <si>
+    <t>20180204000002</t>
+  </si>
+  <si>
+    <t>Johnathann, Henry</t>
   </si>
 </sst>
 </file>
@@ -619,7 +643,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -654,6 +678,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -958,10 +984,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1034,6 +1060,14 @@
         <v>2</v>
       </c>
     </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>152</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1042,7 +1076,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AS35"/>
+  <dimension ref="A1:AS41"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M1" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
       <selection activeCell="W13" sqref="W13"/>
@@ -1298,11 +1332,11 @@
         <v>18</v>
       </c>
       <c r="J7" s="14" t="s">
-        <v>150</v>
+        <v>161</v>
       </c>
       <c r="K7" s="9"/>
       <c r="L7" s="14" t="s">
-        <v>155</v>
+        <v>162</v>
       </c>
       <c r="M7" s="1" t="s">
         <v>121</v>
@@ -1663,10 +1697,10 @@
         <v>129</v>
       </c>
       <c r="W13" s="14" t="s">
-        <v>155</v>
+        <v>163</v>
       </c>
       <c r="X13" s="1" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="Y13" s="1" t="s">
         <v>72</v>
@@ -1687,13 +1721,13 @@
         <v>59</v>
       </c>
       <c r="AE13" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="AF13" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="AG13" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
     </row>
     <row r="14" spans="1:45" x14ac:dyDescent="0.25">
@@ -1800,13 +1834,13 @@
         <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="D19" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="E19" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>48</v>
@@ -1915,13 +1949,13 @@
         <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="D24" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="E24" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>137</v>
@@ -2003,13 +2037,13 @@
         <v>6</v>
       </c>
       <c r="C30" t="s">
-        <v>156</v>
+        <v>164</v>
       </c>
       <c r="D30" t="s">
-        <v>157</v>
+        <v>165</v>
       </c>
       <c r="E30" t="s">
-        <v>158</v>
+        <v>166</v>
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
@@ -2041,13 +2075,9 @@
       <c r="M31" s="19"/>
     </row>
     <row r="33" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A33" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="E33" s="11"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="11"/>
+      <c r="A33" s="3" t="s">
+        <v>152</v>
+      </c>
     </row>
     <row r="34" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A34" s="4" t="s">
@@ -2066,12 +2096,14 @@
         <v>127</v>
       </c>
       <c r="F34" s="6" t="s">
-        <v>21</v>
+        <v>153</v>
       </c>
       <c r="G34" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="H34" s="4"/>
+        <v>155</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>156</v>
+      </c>
       <c r="I34" s="6"/>
       <c r="J34" s="4"/>
       <c r="K34" s="6"/>
@@ -2090,22 +2122,22 @@
       <c r="B35" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C35" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="D35" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>152</v>
+      <c r="C35" t="s">
+        <v>164</v>
+      </c>
+      <c r="D35" t="s">
+        <v>165</v>
+      </c>
+      <c r="E35" t="s">
+        <v>166</v>
       </c>
       <c r="F35" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="G35" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="H35" s="1"/>
+        <v>154</v>
+      </c>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1" t="s">
+        <v>157</v>
+      </c>
       <c r="I35" s="1"/>
       <c r="J35" s="1"/>
       <c r="K35" s="1"/>
@@ -2116,6 +2148,98 @@
       <c r="P35" s="9"/>
       <c r="Q35" s="9"/>
       <c r="R35" s="9"/>
+    </row>
+    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="19"/>
+      <c r="H36" s="19"/>
+      <c r="I36" s="19"/>
+      <c r="J36" s="19"/>
+      <c r="K36" s="19"/>
+      <c r="L36" s="19"/>
+      <c r="M36" s="19"/>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A39" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="E39" s="11"/>
+      <c r="F39" s="11"/>
+      <c r="G39" s="11"/>
+      <c r="H39" s="11"/>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A40" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C40" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>127</v>
+      </c>
+      <c r="F40" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G40" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="H40" s="4"/>
+      <c r="I40" s="6"/>
+      <c r="J40" s="4"/>
+      <c r="K40" s="6"/>
+      <c r="L40" s="4"/>
+      <c r="M40" s="6"/>
+      <c r="N40" s="4"/>
+      <c r="O40" s="6"/>
+      <c r="P40" s="4"/>
+      <c r="Q40" s="6"/>
+      <c r="R40" s="4"/>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A41" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C41" s="10" t="s">
+        <v>158</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+      <c r="L41" s="9"/>
+      <c r="M41" s="1"/>
+      <c r="N41" s="9"/>
+      <c r="O41" s="9"/>
+      <c r="P41" s="9"/>
+      <c r="Q41" s="9"/>
+      <c r="R41" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Changes done in all java class files
Signed-off-by: ACROTECHNOLOGIE\SSinghal <sarthak.singhal8723@gmail.com>
</commit_message>
<xml_diff>
--- a/Acro_Data_Driven_Framework/Acams_Suite_One.xlsx
+++ b/Acro_Data_Driven_Framework/Acams_Suite_One.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="464" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="191">
   <si>
     <t>TCID</t>
   </si>
@@ -489,15 +489,6 @@
     <t>Juan, Jessica</t>
   </si>
   <si>
-    <t>Clarkss</t>
-  </si>
-  <si>
-    <t>20180204000014</t>
-  </si>
-  <si>
-    <t>Gonzalvis, Janis</t>
-  </si>
-  <si>
     <t>CaseCloseFinalComments</t>
   </si>
   <si>
@@ -522,9 +513,6 @@
     <t>80</t>
   </si>
   <si>
-    <t>201802002675</t>
-  </si>
-  <si>
     <t>CC - Bergman, Greg</t>
   </si>
   <si>
@@ -534,21 +522,6 @@
     <t xml:space="preserve">ATC Saved After Client is created. Test </t>
   </si>
   <si>
-    <t>Jackie</t>
-  </si>
-  <si>
-    <t>Jane</t>
-  </si>
-  <si>
-    <t>201802002684</t>
-  </si>
-  <si>
-    <t>20180204000025</t>
-  </si>
-  <si>
-    <t>Jane, Jackie</t>
-  </si>
-  <si>
     <t>FollowUpTest</t>
   </si>
   <si>
@@ -591,14 +564,39 @@
     <t>ClpName</t>
   </si>
   <si>
-    <t>JAMESCARLLLL</t>
+    <t>Surabhi.(Verma1198435</t>
+  </si>
+  <si>
+    <t>201802002703</t>
+  </si>
+  <si>
+    <t>20180204000045</t>
+  </si>
+  <si>
+    <t>Bonds, James</t>
+  </si>
+  <si>
+    <t>Warms</t>
+  </si>
+  <si>
+    <t>Johny</t>
+  </si>
+  <si>
+    <t>201802002704</t>
+  </si>
+  <si>
+    <t>20180204000046</t>
+  </si>
+  <si>
+    <t>Warms, Johny</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1060,8 +1058,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="48.85546875" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="25.28515625" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="48.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="25.28515625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -1138,7 +1136,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="21" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="B10" s="21" t="s">
         <v>2</v>
@@ -1146,7 +1144,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="21" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="B11" s="21" t="s">
         <v>2</v>
@@ -1154,7 +1152,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="21" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="B12" s="21" t="s">
         <v>2</v>
@@ -1162,7 +1160,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="B13" s="21" t="s">
         <v>2</v>
@@ -1170,7 +1168,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="B14" s="21" t="s">
         <v>2</v>
@@ -1178,7 +1176,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="23" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="B15" s="23" t="s">
         <v>2</v>
@@ -1194,54 +1192,54 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AS70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="B70" sqref="B70"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="30.140625" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="33.85546875" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="44" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="35" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="47" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="34.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="15.85546875" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="44.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="26.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="20.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="21.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="25.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="36.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="24.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="23" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="25.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="32" max="32" width="24.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="15.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="24.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="18" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="14.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="20.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="12.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="18.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="22.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="5.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="42" max="42" width="7.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="43" max="43" width="15" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="30.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="33.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="44.0" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="35.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="47.0" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="34.5703125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="44.28515625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="26.42578125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="20.5703125" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="21.140625" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="25.7109375" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="36.7109375" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="24.28515625" collapsed="true"/>
+    <col min="22" max="23" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="25.7109375" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
+    <col min="32" max="32" bestFit="true" customWidth="true" width="24.28515625" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="15.28515625" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="24.7109375" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="36" max="36" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="37" max="37" bestFit="true" customWidth="true" width="20.28515625" collapsed="true"/>
+    <col min="38" max="38" bestFit="true" customWidth="true" width="12.28515625" collapsed="true"/>
+    <col min="39" max="39" bestFit="true" customWidth="true" width="18.5703125" collapsed="true"/>
+    <col min="40" max="40" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
+    <col min="41" max="41" bestFit="true" customWidth="true" width="5.85546875" collapsed="true"/>
+    <col min="42" max="42" bestFit="true" customWidth="true" width="7.7109375" collapsed="true"/>
+    <col min="43" max="43" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:45" x14ac:dyDescent="0.25">
@@ -1448,14 +1446,14 @@
         <v>18</v>
       </c>
       <c r="J7" s="14" t="s">
-        <v>172</v>
+        <v>187</v>
       </c>
       <c r="K7" s="9"/>
       <c r="L7" s="14" t="s">
-        <v>173</v>
+        <v>186</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="N7" s="10" t="s">
         <v>121</v>
@@ -1813,7 +1811,7 @@
         <v>128</v>
       </c>
       <c r="W13" s="14" t="s">
-        <v>157</v>
+        <v>186</v>
       </c>
       <c r="X13" s="1" t="s">
         <v>147</v>
@@ -1837,13 +1835,13 @@
         <v>59</v>
       </c>
       <c r="AE13" t="s">
-        <v>174</v>
+        <v>188</v>
       </c>
       <c r="AF13" t="s">
-        <v>175</v>
+        <v>189</v>
       </c>
       <c r="AG13" t="s">
-        <v>176</v>
+        <v>190</v>
       </c>
     </row>
     <row r="14" spans="1:45" x14ac:dyDescent="0.25">
@@ -1950,13 +1948,13 @@
         <v>6</v>
       </c>
       <c r="C19" t="s">
-        <v>174</v>
+        <v>188</v>
       </c>
       <c r="D19" t="s">
-        <v>175</v>
+        <v>189</v>
       </c>
       <c r="E19" t="s">
-        <v>176</v>
+        <v>190</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>48</v>
@@ -2065,13 +2063,13 @@
         <v>6</v>
       </c>
       <c r="C24" t="s">
-        <v>174</v>
+        <v>188</v>
       </c>
       <c r="D24" t="s">
-        <v>175</v>
+        <v>189</v>
       </c>
       <c r="E24" t="s">
-        <v>176</v>
+        <v>190</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>136</v>
@@ -2153,13 +2151,13 @@
         <v>6</v>
       </c>
       <c r="C30" t="s">
-        <v>174</v>
+        <v>188</v>
       </c>
       <c r="D30" t="s">
-        <v>175</v>
+        <v>189</v>
       </c>
       <c r="E30" t="s">
-        <v>176</v>
+        <v>190</v>
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
@@ -2239,13 +2237,13 @@
         <v>6</v>
       </c>
       <c r="C35" t="s">
-        <v>174</v>
+        <v>188</v>
       </c>
       <c r="D35" t="s">
-        <v>175</v>
+        <v>189</v>
       </c>
       <c r="E35" t="s">
-        <v>176</v>
+        <v>190</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>150</v>
@@ -2359,7 +2357,7 @@
     </row>
     <row r="43" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
     </row>
     <row r="44" spans="1:18" x14ac:dyDescent="0.25">
@@ -2379,7 +2377,7 @@
         <v>126</v>
       </c>
       <c r="F44" s="6" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="G44" s="4"/>
       <c r="H44" s="4"/>
@@ -2402,16 +2400,16 @@
         <v>6</v>
       </c>
       <c r="C45" t="s">
-        <v>174</v>
+        <v>188</v>
       </c>
       <c r="D45" t="s">
-        <v>175</v>
+        <v>189</v>
       </c>
       <c r="E45" t="s">
-        <v>176</v>
+        <v>190</v>
       </c>
       <c r="F45" s="1" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="G45" s="1"/>
       <c r="H45" s="1"/>
@@ -2443,7 +2441,7 @@
     </row>
     <row r="48" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
     </row>
     <row r="49" spans="1:18" x14ac:dyDescent="0.25">
@@ -2463,10 +2461,10 @@
         <v>126</v>
       </c>
       <c r="F49" s="6" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="H49" s="4"/>
       <c r="I49" s="6"/>
@@ -2487,20 +2485,20 @@
       <c r="B50" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C50" s="20" t="s">
-        <v>168</v>
+      <c r="C50" t="s">
+        <v>188</v>
       </c>
       <c r="D50" t="s">
-        <v>158</v>
+        <v>189</v>
       </c>
       <c r="E50" t="s">
-        <v>159</v>
+        <v>190</v>
       </c>
       <c r="F50" s="10" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="H50" s="1"/>
       <c r="I50" s="1"/>
@@ -2531,7 +2529,7 @@
     </row>
     <row r="53" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="54" spans="1:18" x14ac:dyDescent="0.25">
@@ -2580,22 +2578,22 @@
         <v>6</v>
       </c>
       <c r="C55" t="s">
-        <v>174</v>
+        <v>188</v>
       </c>
       <c r="D55" t="s">
-        <v>175</v>
+        <v>189</v>
       </c>
       <c r="E55" t="s">
-        <v>176</v>
+        <v>190</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="G55" s="10" t="s">
         <v>121</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="I55" s="10" t="s">
         <v>120</v>
@@ -2627,7 +2625,7 @@
     </row>
     <row r="59" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
     </row>
     <row r="60" spans="1:18" x14ac:dyDescent="0.25">
@@ -2650,10 +2648,10 @@
         <v>115</v>
       </c>
       <c r="G60" s="6" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="H60" s="6" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="I60" s="6"/>
       <c r="J60" s="4"/>
@@ -2674,22 +2672,22 @@
         <v>6</v>
       </c>
       <c r="C61" t="s">
-        <v>174</v>
+        <v>188</v>
       </c>
       <c r="D61" t="s">
-        <v>175</v>
+        <v>189</v>
       </c>
       <c r="E61" t="s">
-        <v>176</v>
+        <v>190</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="G61" s="10" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="I61" s="10"/>
       <c r="J61" s="1"/>
@@ -2719,7 +2717,7 @@
     </row>
     <row r="64" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
     </row>
     <row r="65" spans="1:18" x14ac:dyDescent="0.25">
@@ -2742,10 +2740,10 @@
         <v>115</v>
       </c>
       <c r="G65" s="6" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="H65" s="6" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="I65" s="6"/>
       <c r="J65" s="4"/>
@@ -2766,22 +2764,22 @@
         <v>6</v>
       </c>
       <c r="C66" t="s">
-        <v>174</v>
+        <v>188</v>
       </c>
       <c r="D66" t="s">
+        <v>189</v>
+      </c>
+      <c r="E66" t="s">
+        <v>190</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="G66" s="10" t="s">
+        <v>170</v>
+      </c>
+      <c r="H66" s="1" t="s">
         <v>175</v>
-      </c>
-      <c r="E66" t="s">
-        <v>176</v>
-      </c>
-      <c r="F66" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="G66" s="10" t="s">
-        <v>179</v>
-      </c>
-      <c r="H66" s="1" t="s">
-        <v>184</v>
       </c>
       <c r="I66" s="10"/>
       <c r="J66" s="1"/>
@@ -2796,7 +2794,7 @@
     </row>
     <row r="68" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
     </row>
     <row r="69" spans="1:18" x14ac:dyDescent="0.25">
@@ -2807,7 +2805,7 @@
         <v>3</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="D69" s="6" t="s">
         <v>4</v>
@@ -2816,7 +2814,7 @@
         <v>5</v>
       </c>
       <c r="F69" s="6" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="G69" s="6"/>
       <c r="H69" s="6"/>
@@ -2831,24 +2829,24 @@
       <c r="Q69" s="6"/>
       <c r="R69" s="4"/>
     </row>
-    <row r="70" spans="1:18" ht="30" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C70" s="7" t="s">
-        <v>187</v>
+      <c r="C70" t="s">
+        <v>178</v>
       </c>
       <c r="D70" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="E70" s="20" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="G70" s="10"/>
       <c r="H70" s="1"/>
@@ -2879,44 +2877,44 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="39.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="17" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="15" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="20.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="27" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="31.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="5.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="7.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="7.140625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="11" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="22" max="22" width="6" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="23" max="23" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="24" max="24" width="7.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="25" max="25" width="12" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="26" max="26" width="8" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="27" max="27" width="9" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="28" max="28" width="14" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="29" max="29" width="8.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="30" max="30" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="31" max="31" width="8.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="33" max="33" width="11.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="34" max="34" width="14.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="35" max="35" width="8.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="36" max="36" width="18.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="37" max="37" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="38" max="38" width="8.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="39" max="39" width="20.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="40" max="40" width="4.5703125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="41" max="41" width="5.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="39.140625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="8.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="20.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="27.0" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="31.7109375" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="8.5703125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="5.85546875" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="7.7109375" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="7.140625" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="6.0" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
+    <col min="29" max="29" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="8.5703125" collapsed="true"/>
+    <col min="36" max="36" bestFit="true" customWidth="true" width="18.85546875" collapsed="true"/>
+    <col min="37" max="37" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="38" max="38" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="39" max="39" bestFit="true" customWidth="true" width="20.7109375" collapsed="true"/>
+    <col min="40" max="40" bestFit="true" customWidth="true" width="4.5703125" collapsed="true"/>
+    <col min="41" max="41" bestFit="true" customWidth="true" width="5.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:41" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
updated on 28-feb Signed-off-by: ACROTECHNOLOGIE\SSinghal <sarthak.singhal8723@gmail.com>
</commit_message>
<xml_diff>
--- a/Acro_Data_Driven_Framework/Acams_Suite_One.xlsx
+++ b/Acro_Data_Driven_Framework/Acams_Suite_One.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11655" windowHeight="4650" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20460" windowHeight="7680" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="191">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="190">
   <si>
     <t>TCID</t>
   </si>
@@ -552,43 +552,40 @@
     <t>Url</t>
   </si>
   <si>
-    <t>http://203.122.16.47/xrm_qa/newuserlogin.aspx</t>
-  </si>
-  <si>
-    <t>acroxrm</t>
-  </si>
-  <si>
-    <t>444444</t>
-  </si>
-  <si>
     <t>ClpName</t>
   </si>
   <si>
-    <t>Surabhi.(Verma1198435</t>
-  </si>
-  <si>
-    <t>201802002703</t>
-  </si>
-  <si>
-    <t>20180204000045</t>
-  </si>
-  <si>
-    <t>Bonds, James</t>
-  </si>
-  <si>
-    <t>Warms</t>
-  </si>
-  <si>
-    <t>Johny</t>
-  </si>
-  <si>
-    <t>201802002704</t>
-  </si>
-  <si>
-    <t>20180204000046</t>
-  </si>
-  <si>
-    <t>Warms, Johny</t>
+    <t>Surabhi.(Verma1148419</t>
+  </si>
+  <si>
+    <t>201802002712</t>
+  </si>
+  <si>
+    <t>20180204000054</t>
+  </si>
+  <si>
+    <t>Thor, James</t>
+  </si>
+  <si>
+    <t>123456</t>
+  </si>
+  <si>
+    <t>xrmsecurity</t>
+  </si>
+  <si>
+    <t>Samuel</t>
+  </si>
+  <si>
+    <t>Willliams</t>
+  </si>
+  <si>
+    <t>201802002726</t>
+  </si>
+  <si>
+    <t>20180204000069</t>
+  </si>
+  <si>
+    <t>Willliams, Samuel</t>
   </si>
 </sst>
 </file>
@@ -1192,8 +1189,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AS70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScale="68" zoomScaleNormal="68" workbookViewId="0">
+      <selection activeCell="W13" sqref="W13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1446,7 +1443,7 @@
         <v>18</v>
       </c>
       <c r="J7" s="14" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="K7" s="9"/>
       <c r="L7" s="14" t="s">
@@ -1835,13 +1832,13 @@
         <v>59</v>
       </c>
       <c r="AE13" t="s">
+        <v>187</v>
+      </c>
+      <c r="AF13" t="s">
         <v>188</v>
       </c>
-      <c r="AF13" t="s">
+      <c r="AG13" t="s">
         <v>189</v>
-      </c>
-      <c r="AG13" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="14" spans="1:45" x14ac:dyDescent="0.25">
@@ -1948,13 +1945,13 @@
         <v>6</v>
       </c>
       <c r="C19" t="s">
+        <v>187</v>
+      </c>
+      <c r="D19" t="s">
         <v>188</v>
       </c>
-      <c r="D19" t="s">
+      <c r="E19" t="s">
         <v>189</v>
-      </c>
-      <c r="E19" t="s">
-        <v>190</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>48</v>
@@ -2063,13 +2060,13 @@
         <v>6</v>
       </c>
       <c r="C24" t="s">
+        <v>187</v>
+      </c>
+      <c r="D24" t="s">
         <v>188</v>
       </c>
-      <c r="D24" t="s">
+      <c r="E24" t="s">
         <v>189</v>
-      </c>
-      <c r="E24" t="s">
-        <v>190</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>136</v>
@@ -2151,13 +2148,13 @@
         <v>6</v>
       </c>
       <c r="C30" t="s">
+        <v>187</v>
+      </c>
+      <c r="D30" t="s">
         <v>188</v>
       </c>
-      <c r="D30" t="s">
+      <c r="E30" t="s">
         <v>189</v>
-      </c>
-      <c r="E30" t="s">
-        <v>190</v>
       </c>
       <c r="F30" s="1"/>
       <c r="G30" s="1"/>
@@ -2237,13 +2234,13 @@
         <v>6</v>
       </c>
       <c r="C35" t="s">
+        <v>187</v>
+      </c>
+      <c r="D35" t="s">
         <v>188</v>
       </c>
-      <c r="D35" t="s">
+      <c r="E35" t="s">
         <v>189</v>
-      </c>
-      <c r="E35" t="s">
-        <v>190</v>
       </c>
       <c r="F35" s="1" t="s">
         <v>150</v>
@@ -2400,13 +2397,13 @@
         <v>6</v>
       </c>
       <c r="C45" t="s">
+        <v>187</v>
+      </c>
+      <c r="D45" t="s">
         <v>188</v>
       </c>
-      <c r="D45" t="s">
+      <c r="E45" t="s">
         <v>189</v>
-      </c>
-      <c r="E45" t="s">
-        <v>190</v>
       </c>
       <c r="F45" s="1" t="s">
         <v>158</v>
@@ -2486,13 +2483,13 @@
         <v>6</v>
       </c>
       <c r="C50" t="s">
+        <v>187</v>
+      </c>
+      <c r="D50" t="s">
         <v>188</v>
       </c>
-      <c r="D50" t="s">
+      <c r="E50" t="s">
         <v>189</v>
-      </c>
-      <c r="E50" t="s">
-        <v>190</v>
       </c>
       <c r="F50" s="10" t="s">
         <v>164</v>
@@ -2578,13 +2575,13 @@
         <v>6</v>
       </c>
       <c r="C55" t="s">
+        <v>187</v>
+      </c>
+      <c r="D55" t="s">
         <v>188</v>
       </c>
-      <c r="D55" t="s">
+      <c r="E55" t="s">
         <v>189</v>
-      </c>
-      <c r="E55" t="s">
-        <v>190</v>
       </c>
       <c r="F55" s="1" t="s">
         <v>165</v>
@@ -2672,13 +2669,13 @@
         <v>6</v>
       </c>
       <c r="C61" t="s">
+        <v>187</v>
+      </c>
+      <c r="D61" t="s">
         <v>188</v>
       </c>
-      <c r="D61" t="s">
+      <c r="E61" t="s">
         <v>189</v>
-      </c>
-      <c r="E61" t="s">
-        <v>190</v>
       </c>
       <c r="F61" s="1" t="s">
         <v>165</v>
@@ -2764,13 +2761,13 @@
         <v>6</v>
       </c>
       <c r="C66" t="s">
+        <v>187</v>
+      </c>
+      <c r="D66" t="s">
         <v>188</v>
       </c>
-      <c r="D66" t="s">
+      <c r="E66" t="s">
         <v>189</v>
-      </c>
-      <c r="E66" t="s">
-        <v>190</v>
       </c>
       <c r="F66" s="1" t="s">
         <v>165</v>
@@ -2814,7 +2811,7 @@
         <v>5</v>
       </c>
       <c r="F69" s="6" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="G69" s="6"/>
       <c r="H69" s="6"/>
@@ -2836,17 +2833,14 @@
       <c r="B70" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C70" t="s">
-        <v>178</v>
-      </c>
       <c r="D70" t="s">
+        <v>184</v>
+      </c>
+      <c r="E70" s="20" t="s">
+        <v>183</v>
+      </c>
+      <c r="F70" s="1" t="s">
         <v>179</v>
-      </c>
-      <c r="E70" s="20" t="s">
-        <v>180</v>
-      </c>
-      <c r="F70" s="1" t="s">
-        <v>182</v>
       </c>
       <c r="G70" s="10"/>
       <c r="H70" s="1"/>

</xml_diff>